<commit_message>
a stable version of discourse parser
</commit_message>
<xml_diff>
--- a/data/连词词表计算/连词非连词个数.xlsx
+++ b/data/连词词表计算/连词非连词个数.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -1021,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A212" sqref="A212:XFD212"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3360,30 +3358,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>